<commit_message>
rename system name in figure files
</commit_message>
<xml_diff>
--- a/draft/include/figure/deepDiveExper.xlsx
+++ b/draft/include/figure/deepDiveExper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="32160" yWindow="2080" windowWidth="29020" windowHeight="19840" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,6 @@
     <t>IDEAL</t>
   </si>
   <si>
-    <t>KRD</t>
-  </si>
-  <si>
     <t>OnlyPos</t>
   </si>
   <si>
@@ -37,6 +34,9 @@
   </si>
   <si>
     <t>1000 articles</t>
+  </si>
+  <si>
+    <t>RuDiK</t>
   </si>
 </sst>
 </file>
@@ -293,7 +293,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>KRD</c:v>
+                  <c:v>RuDiK</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -772,11 +772,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2141515560"/>
-        <c:axId val="-2142082600"/>
+        <c:axId val="310397032"/>
+        <c:axId val="422887992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2141515560"/>
+        <c:axId val="310397032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -797,12 +797,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2142082600"/>
+        <c:crossAx val="422887992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2142082600"/>
+        <c:axId val="422887992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -824,7 +824,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2141515560"/>
+        <c:crossAx val="310397032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1023,7 +1023,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>KRD</c:v>
+                  <c:v>RuDiK</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1505,11 +1505,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2133773240"/>
-        <c:axId val="-2133772168"/>
+        <c:axId val="311129592"/>
+        <c:axId val="423565224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2133773240"/>
+        <c:axId val="311129592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1530,12 +1530,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133772168"/>
+        <c:crossAx val="423565224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2133772168"/>
+        <c:axId val="423565224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1557,7 +1557,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133773240"/>
+        <c:crossAx val="311129592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1989,8 +1989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A9:M62"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A31" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="N65" sqref="N65"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A43" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="S66" sqref="S66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2000,7 +2000,7 @@
   <sheetData>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -2084,7 +2084,7 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -2116,7 +2116,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -2133,7 +2133,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14">
         <v>4.4971381847899996E-3</v>
@@ -2168,7 +2168,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -2203,7 +2203,7 @@
     </row>
     <row r="56" spans="1:13">
       <c r="A56" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:13">
@@ -2287,7 +2287,7 @@
     </row>
     <row r="59" spans="1:13">
       <c r="A59" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C59">
         <v>2.6097271648870001E-2</v>
@@ -2322,7 +2322,7 @@
     </row>
     <row r="60" spans="1:13">
       <c r="A60" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I60">
         <v>1</v>
@@ -2339,7 +2339,7 @@
     </row>
     <row r="61" spans="1:13">
       <c r="A61" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C61">
         <v>2.8204975951999999E-4</v>
@@ -2374,7 +2374,7 @@
     </row>
     <row r="62" spans="1:13">
       <c r="A62" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C62">
         <v>2.0554066130500002E-3</v>

</xml_diff>